<commit_message>
Update Copy of 2022April Sprint Test cases
</commit_message>
<xml_diff>
--- a/Copy of 2022April Sprint Test cases.xlsx
+++ b/Copy of 2022April Sprint Test cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\561625\Documents\GitHub\UiPath-Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988E5840-20DD-461C-B7E6-76A14BAA619A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F0C736-BE47-4721-BD40-229095FA4BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="510" windowWidth="25545" windowHeight="15225" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
+    <workbookView xWindow="10140" yWindow="1110" windowWidth="17655" windowHeight="14490" xr2:uid="{A2A8D2E7-EC1F-4C5E-B330-8D00094F85E8}"/>
   </bookViews>
   <sheets>
     <sheet name="RPA Test Cases" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>SR#</t>
   </si>
@@ -202,6 +202,45 @@
   </si>
   <si>
     <t>not added to queue by Dispatcher</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991047</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: TESTING</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991048</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991040</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991041</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991044</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991046</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991002</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 991045</t>
+  </si>
+  <si>
+    <t>Reason: No matching Account Number on the lookup table. Account Number: 533704</t>
+  </si>
+  <si>
+    <t>Success, CCR</t>
+  </si>
+  <si>
+    <t>Success, Assign To</t>
+  </si>
+  <si>
+    <t>SR0003015462</t>
   </si>
 </sst>
 </file>
@@ -626,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2626AB73-D654-434C-9659-C4D28008D556}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +746,9 @@
       <c r="F3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -729,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -751,7 +792,9 @@
       <c r="F5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -772,7 +815,9 @@
       <c r="F6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -793,7 +838,9 @@
       <c r="F7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -814,7 +861,9 @@
       <c r="F8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -835,7 +884,9 @@
       <c r="F9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -856,7 +907,9 @@
       <c r="F10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -877,7 +930,9 @@
       <c r="F11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -896,7 +951,9 @@
       <c r="F12" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -915,10 +972,14 @@
       <c r="F13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B14" s="8" t="s">
         <v>52</v>
       </c>
@@ -932,7 +993,9 @@
       <c r="F14" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>